<commit_message>
test file is added
</commit_message>
<xml_diff>
--- a/KFCSAMavenProject/TestData/TestData.xlsx
+++ b/KFCSAMavenProject/TestData/TestData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
   <si>
     <t>Chrome</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>validateInValidaLogin</t>
+  </si>
+  <si>
+    <t>Arvind-10.Kumar-10@cognizant.com</t>
   </si>
 </sst>
 </file>
@@ -414,16 +417,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="47.5703125" bestFit="1" customWidth="1"/>
   </cols>
@@ -500,14 +503,29 @@
         <v>7</v>
       </c>
     </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B1" r:id="rId1"/>
     <hyperlink ref="C2" r:id="rId2"/>
     <hyperlink ref="C4" r:id="rId3"/>
     <hyperlink ref="C5" r:id="rId4"/>
+    <hyperlink ref="C6" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>